<commit_message>
try to fix after google maps changed html and css
</commit_message>
<xml_diff>
--- a/Shrimp.xlsx
+++ b/Shrimp.xlsx
@@ -763,22 +763,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SeaFood Bar&amp;Market</t>
+          <t>Mango Mama</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rogowska 50B, 54-438 Wrocław </t>
+          <t xml:space="preserve">Świętego Mikołaja 18, 50-128 Wrocław </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">22 671 25 75 </t>
+          <t xml:space="preserve">535 653 692 </t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve">seafoodbar.pl </t>
+          <t xml:space="preserve">mangomama.pl </t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -790,54 +790,54 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Shrimp Nature</t>
+          <t>Wok in</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sokolnicza 7/17, 53-671 Wrocław </t>
+          <t xml:space="preserve">Sukiennice 1/2, 50-116 Wrocław </t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">511 583 730 </t>
+          <t xml:space="preserve">781 026 510 </t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve">wokin.pl </t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 3,9</t>
+          <t xml:space="preserve"> 4,6</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Sea-Food Crab Meat Sokolnicza 7/17 Wrocław</t>
+          <t>Vertigo Jazz Club &amp; Restaurant</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Klimasa 37F, 50-515 Wrocław </t>
+          <t xml:space="preserve">Oławska 13, 50-123 Wrocław </t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">692 145 513 </t>
+          <t xml:space="preserve">71 718 25 81 </t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve">vertigojazz.pl </t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5,0</t>
+          <t xml:space="preserve"> 4,7</t>
         </is>
       </c>
     </row>

</xml_diff>